<commit_message>
dankuzone /w DAIC - evidence submission for tasks A1-A6
</commit_message>
<xml_diff>
--- a/DAICers/evidence.xlsx
+++ b/DAICers/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GoogleDrive\Private\DAIC_GmbH\14_Projects\GameOfNfts\Saikoro no tori\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67790315-8E14-4615-B56D-52B98D523EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAF6B29-03EB-47CD-AF78-83CD73A7F55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2772" yWindow="1596" windowWidth="24276" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28608" yWindow="1872" windowWidth="28080" windowHeight="12312" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="42">
   <si>
     <t>TxHash</t>
   </si>
@@ -79,24 +79,6 @@
     <t>nft id</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -143,6 +125,51 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>6779BEE088F3AFD8AE23BF07FA7ED89B061021A310F055CD6DEB164168A14221</t>
+  </si>
+  <si>
+    <t>saikoronotori</t>
+  </si>
+  <si>
+    <t>71BE265098FCB57E7DFE83559E4FC350B742E7E4BA915FFEAF799295FAE0223E</t>
+  </si>
+  <si>
+    <t>saikoronotori01</t>
+  </si>
+  <si>
+    <t>DA82E9D40F97180067FB64D7F9BF84441B7F1DC222F91DE3E76D427651B8FC07</t>
+  </si>
+  <si>
+    <t>saikoronotori02</t>
+  </si>
+  <si>
+    <t>BCC192B1D57C88A0598B001CF389C4542504196758E5E6C8CC6ACFF3EE6DD73F</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>juno14acs4qq74005wyucgv06lqzje8er88753rn47fdvqpf4gwxf92ysj9hz8n</t>
+  </si>
+  <si>
+    <t>998B1DF93777728F3B76B5FBA0213AA25B76BEA4296946A2BD57F76A9085E4A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>ibc/CCDF0E008EB8940349BAD859F198A7A07A52BEC85CC5FBC53AC80F81FDEBBB85</t>
+  </si>
+  <si>
+    <t>3538EFA85341F38E0EC645FF5D7396AF33A4CC3FB0CA92E50D5605BCFC781F69</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>657FACAED665C6C58BD896D8EFE307491980209D029400BF08A1A0B012B067C4</t>
   </si>
 </sst>
 </file>
@@ -537,8 +564,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,54 +582,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="H2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1064,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1054,10 +1083,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1298,9 +1327,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1321,13 +1352,24 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1342,7 +1384,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1367,16 +1411,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1435,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1416,16 +1462,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1486,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1465,16 +1513,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1489,7 +1537,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1515,16 +1565,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tasks A7-A20, B1 and B2
</commit_message>
<xml_diff>
--- a/DAICers/evidence.xlsx
+++ b/DAICers/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GoogleDrive\Private\DAIC_GmbH\14_Projects\GameOfNfts\Saikoro no tori\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAF6B29-03EB-47CD-AF78-83CD73A7F55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A32954-CB46-4E5C-8806-2B356734ACD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28608" yWindow="1872" windowWidth="28080" windowHeight="12312" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25395" yWindow="4050" windowWidth="22710" windowHeight="12315" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -170,6 +155,171 @@
   </si>
   <si>
     <t>657FACAED665C6C58BD896D8EFE307491980209D029400BF08A1A0B012B067C4</t>
+  </si>
+  <si>
+    <t>ibc/D4B9CD88608C3A19CEE6A0E332708C2E933D1425295D03B1F1C3B97EEB411630</t>
+  </si>
+  <si>
+    <t>saikoronotori03</t>
+  </si>
+  <si>
+    <t>ibc/2E2542B644F7C8828C5602E275272EA682C574AC9713AAE72788274369ACB89A</t>
+  </si>
+  <si>
+    <t>saikoronotori04</t>
+  </si>
+  <si>
+    <t>ibc/84FF66A76EF3C96171764388296D40BD31EAA8890C7B5FDC68D89CA1246D57BF</t>
+  </si>
+  <si>
+    <t>saikoronotori05</t>
+  </si>
+  <si>
+    <t>ibc/0857EA36F7F860891A1E16109B6429366BFE121B5575DC0161ECE0CA2B080EE9</t>
+  </si>
+  <si>
+    <t>saikoronotori06</t>
+  </si>
+  <si>
+    <t>ibc/551AD1DE870A18764467E8BA019C197C29BE4E25F1EBF2E96B55502C541D7713</t>
+  </si>
+  <si>
+    <t>saikoronotori07</t>
+  </si>
+  <si>
+    <t>E3A076F07CB2B38B7CE9B36A119EEEDBBB9D24E87D5AAD4CB123F8D1A8171911</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>40C6EBA023C901032E68C2145E8292D37CBF247ED91A62EC5C5FE92A906FA90C</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>1A603ACF93EB84A50BE4B13E9D1EC7F8893748C2C10A244CC06892B6C8898EDC</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>C6893C91BD23BB71239853B8D5C220C712B4A81BDAD96F1B5DDF09C95E0713C2</t>
+  </si>
+  <si>
+    <t>ibc/27AB938F6C18C18BCDD7343B85A937BA9CB4054DEE62B0B8EAE59BC24B9B7410</t>
+  </si>
+  <si>
+    <t>saikoronotori09</t>
+  </si>
+  <si>
+    <t>FA1456B2319CB5D55CD111780298510193AD390C95819A855EA4174C0B5DBBBC</t>
+  </si>
+  <si>
+    <t>DA2A691ECA506166F5A5318C1E699DF6AB18C3C724A1E7F970E5C83DD7F97DDF</t>
+  </si>
+  <si>
+    <t>7FDAFA03B85D1EA0B66D4FF248FD1926BC907B1516FFF463B3031205522179DB</t>
+  </si>
+  <si>
+    <t>98A9F3462DD5709363A02906B1280C1638A22972004B4588BD5C019F51F5AB4B</t>
+  </si>
+  <si>
+    <t>96D9CC9D755D41CA8482D40C03EA220154D4FFD65F8DB6A981B2C63F4728CF88</t>
+  </si>
+  <si>
+    <t>0B4929C2A955F22C824FE3A89B72AAF335659312E988A68730D88585DFF0E932</t>
+  </si>
+  <si>
+    <t>FF07D6E3E924C7380983F345F8C1F22EC1919B14C17675A7E23CD1FA9FED66FD</t>
+  </si>
+  <si>
+    <t>B9BCFF7A6CD108329599CB8A7C6E4D0539D01076100E4A72971847ED5F06DEF0</t>
+  </si>
+  <si>
+    <t>A454476A148B6682745A339ACA55BCCBA7D847C30538CCF3C9D5FDFBF22F14C5</t>
+  </si>
+  <si>
+    <t>16493B721E8D75219C366F5190010A3409FB63E6178F61F003C55BADD410E8E1</t>
+  </si>
+  <si>
+    <t>B7C525BB16D8B25E2A227AC6425B899ED6CD89C6C90B025936584EFA48D7760C</t>
+  </si>
+  <si>
+    <t>2BA1076926E3C4433F58FD651EBA969BD2AFC485BC3F0B53AC71E7AD4F698745</t>
+  </si>
+  <si>
+    <t>26FBD3F2E03AD6AAF321369E5FE805879F0EB4B129906B1B4B64EBEB3D6C7095</t>
+  </si>
+  <si>
+    <t>F00B4230692D81C30DC2672283C7506DAF1F55EFFBACA86DA16F9C69B4895C8E</t>
+  </si>
+  <si>
+    <t>F53305BC62667549816433F80B98380AB016D28A60419E66A9309CF24FDF8073</t>
+  </si>
+  <si>
+    <t>F17B079AC445C40EE3132B021A4E7E0F54856F03E55DD739921786AFD33C5861</t>
+  </si>
+  <si>
+    <t>B6FCFAA5E3292A201B6B14C7EC572D6A65F9B8901BD0ED393E926120D9425468</t>
+  </si>
+  <si>
+    <t>8166DBB5055A456E544EBC089BDC240E81E9EFBDF7D60745568D6C42DC76123B</t>
+  </si>
+  <si>
+    <t>576DD0EDE02D6633EC31623A71F2C7A9262364C86BFC9685A41F52D9331C0B02</t>
+  </si>
+  <si>
+    <t>91AA4866581BB831252FC052E884AF79A5C6FFD03E88DFFE5BCB4F8ADA96E965</t>
+  </si>
+  <si>
+    <t>23804FECD9B90566550E734B306EF713C2C45437F11627C2E1C27FA3ACC751F5</t>
+  </si>
+  <si>
+    <t>64FA1DFE9EC49976B34DF64C6D76222E69153E80730774B0EEBF075158E7D26B</t>
+  </si>
+  <si>
+    <t>511C36B80C458CBD068AB4E820F1EB441F64C1C4BB3B13C759E5B48A1DAF6552</t>
+  </si>
+  <si>
+    <t>58DC7EF4ABF1DFC1972488743B601962FEB316CAA69C0F8C22AAE26714E4B9AF</t>
+  </si>
+  <si>
+    <t>52D1826E5AB454457648DE65FD56E8674C4163BCEEF8F9A377034B71FE5D832B</t>
+  </si>
+  <si>
+    <t>800A77F285ABB232852BB7BA328AF1E499D0DDF319B32616051A20DD5AA9F26B</t>
+  </si>
+  <si>
+    <t>94B5312D8070C0F52E940D4B80AFCA3FBF58A54C6C4FAABA2B68496F40AFA8F3</t>
+  </si>
+  <si>
+    <t>E034AE627AD30E390590C885BC69F518A025FA45E44380A7DA36206E90B90230</t>
+  </si>
+  <si>
+    <t>6F2A343CC343FAE4ED7ED9781BDCB21D0CF2F38A744454BBD3960C1353C0B1D9</t>
+  </si>
+  <si>
+    <t>6EB448510BC15E323F0F1DAE6B68C4C335E3D3FC19A9319B914BFE1F60040749</t>
+  </si>
+  <si>
+    <t>A9C6D9A6E57112D3CFF529A8D62276447976C57A62335BDF970924BD1F1D3F77</t>
+  </si>
+  <si>
+    <t>6BE30AB96E46B8324ACCAD23456E3960CD8E4BBE2C349DCA1315CB39D1E8E1FC</t>
+  </si>
+  <si>
+    <t>0DED4D15FA2B5F2F559625664D6F5EB5547B5538C7172D76415A039156542109</t>
+  </si>
+  <si>
+    <t>EE40EA8483C916C8638C90EA5C5C140D4ED91E4B8AE602A0C4F2EB3267045716</t>
+  </si>
+  <si>
+    <t>4AEA5B140BD1BB0010F52573A34C37110FE4894512CFE173CF77EE445875FCC9</t>
+  </si>
+  <si>
+    <t>27C1DF5E5F5E74D86D05D8433C313A1256DA62A038F08B7DF808A026BBF14922</t>
   </si>
 </sst>
 </file>
@@ -243,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,6 +405,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -582,54 +735,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +797,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -654,18 +809,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +835,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -690,18 +847,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +873,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -726,18 +885,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -752,7 +911,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -762,18 +923,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -786,9 +947,197 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -806,35 +1155,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -852,35 +1217,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -898,35 +1279,88 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -944,35 +1378,67 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -990,195 +1456,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1193,6 +1514,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1220,8 +1613,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1254,74 +1647,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
@@ -1344,32 +1669,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1400,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1411,16 +1736,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1761,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,10 +1776,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1462,16 +1787,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1502,10 +1827,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1513,16 +1838,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1537,7 +1862,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1554,10 +1879,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1565,31 +1890,71 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1599,54 +1964,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DAICers Evidences for B5, B6, B7
</commit_message>
<xml_diff>
--- a/DAICers/evidence.xlsx
+++ b/DAICers/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GoogleDrive\Private\DAIC_GmbH\14_Projects\GameOfNfts\Saikoro no tori\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A32954-CB46-4E5C-8806-2B356734ACD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7CD745-0A59-45B1-B142-5E575DD1B39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25395" yWindow="4050" windowWidth="22710" windowHeight="12315" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="78300" yWindow="-4545" windowWidth="16485" windowHeight="9855" firstSheet="16" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -320,6 +315,24 @@
   </si>
   <si>
     <t>27C1DF5E5F5E74D86D05D8433C313A1256DA62A038F08B7DF808A026BBF14922</t>
+  </si>
+  <si>
+    <t>686B8A73A286259B2158D0EA1F60C51AB92E732621B4A6D0E5A944D8B93D9598</t>
+  </si>
+  <si>
+    <t>D112F6BC04A50C3E9BB15D2DC1F6347AB5C53B606D154260631CD80CD1FD80F3</t>
+  </si>
+  <si>
+    <t>3EF9BA7A3D56435D8F7A65673C1816106F89D26F7314BA733EDD19055406F544</t>
+  </si>
+  <si>
+    <t>4CA55ADCB34CD824380FB3199CC4BB3932D26A4C4D5A04D921368A4F028A95F0</t>
+  </si>
+  <si>
+    <t>E0895C5AC1B4D44B48CCA88D2BC5BAFA39A1507363C0F525E97E602D75726F3F</t>
+  </si>
+  <si>
+    <t>79EC180F0D36F7774EBA0FA5BB81F7320502C7426B687EDB2072C9343F8FD03D</t>
   </si>
 </sst>
 </file>
@@ -393,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -405,9 +418,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -735,54 +745,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -809,10 +819,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -828,15 +876,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,10 +895,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -866,15 +952,201 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,34 +1157,58 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,61 +1219,262 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="82.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -985,440 +1482,31 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="82.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="51.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>79</v>
+      <c r="A7" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -1429,84 +1517,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
@@ -1530,12 +1540,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1550,8 +1560,44 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1579,14 +1625,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1600,27 +1648,29 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9443CA73-C1AD-4BA2-B613-7E483A9AC869}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1634,12 +1684,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1669,32 +1719,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1725,27 +1775,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1776,27 +1826,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1827,27 +1877,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1879,27 +1929,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1926,10 +1976,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1943,42 +2031,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>